<commit_message>
aggiornamento 2026 01 12 17:37
</commit_message>
<xml_diff>
--- a/AntonioCristiano/Fust1_mappatura_10_Mandich_Riccardo.xlsx
+++ b/AntonioCristiano/Fust1_mappatura_10_Mandich_Riccardo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RickyMandich\PROJECT\appuntiITS\AntonioCristiano\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0026AE81-8A63-44B7-AD37-1B7C5D22E2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F21F563-2861-4E38-B5E6-A6634D65783E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
   <si>
     <t>STUDENTE:</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Developer</t>
   </si>
   <si>
-    <t xml:space="preserve">                          </t>
-  </si>
-  <si>
     <t>345 702 8296 (trovato su maps, nel sito non lo trovo)</t>
   </si>
   <si>
@@ -130,6 +127,72 @@
   </si>
   <si>
     <t>AI &amp; Data Automation, Buisness Strategy and execution, Cloud Operation, Customer experience transformation, Cybersecurity, Enterprise Process Optimisation and automation, People and organisation</t>
+  </si>
+  <si>
+    <t>Vai software</t>
+  </si>
+  <si>
+    <t>Gioco a carte con un dipendente dell'azienda</t>
+  </si>
+  <si>
+    <t>FINANCE: sono specializzati nel settore finanziario e nella gestione dei crediti, SYSTEM INTEGRATION: collaborano nella migrazione alle nuove tecnologie, RICERCA E SVILUPPO: lavorano all'integrazione di modelli generativi per rendere chiari i vari assaggi a tutti</t>
+  </si>
+  <si>
+    <t>https://www.vaisoftware.it</t>
+  </si>
+  <si>
+    <t>Padova</t>
+  </si>
+  <si>
+    <t>049 807 4243</t>
+  </si>
+  <si>
+    <t>info@vaisoftware.it</t>
+  </si>
+  <si>
+    <t>con i mezzi pubblici</t>
+  </si>
+  <si>
+    <t>il sito non dispone di questa pagina</t>
+  </si>
+  <si>
+    <t>Outsourcing IT, servizi digitali e backoffice per intermediari finanziari (Confidi, PMI, finanza). Consulenza, BPO, automazione dei processi, sistemi applicativi e customer experience.</t>
+  </si>
+  <si>
+    <t>il padre di una ragazza del gruppo giovanile di tiro con l'arco è un dipendente dell'azienda</t>
+  </si>
+  <si>
+    <t>Galileo Network</t>
+  </si>
+  <si>
+    <t>https://galileonetwork.it/</t>
+  </si>
+  <si>
+    <t>049 295 7811</t>
+  </si>
+  <si>
+    <t>info@galileonetwork.it</t>
+  </si>
+  <si>
+    <t>CFO (Chief Financial Officer)</t>
+  </si>
+  <si>
+    <t>mapo studio</t>
+  </si>
+  <si>
+    <t>ho farso un corso sull'AI da loro l'anno scorso (organizzato tramite coges don milani)</t>
+  </si>
+  <si>
+    <t>Studio digitale e di comunicazione: sviluppo siti web e piattaforme digitali, e-commerce, app, branding, marketing digitale, produzione video e fotografia.</t>
+  </si>
+  <si>
+    <t>https://www.mapostudio.com/</t>
+  </si>
+  <si>
+    <t>info@mapostudio.com</t>
+  </si>
+  <si>
+    <t>041 5312831</t>
   </si>
 </sst>
 </file>
@@ -291,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -308,6 +371,12 @@
     <xf numFmtId="49" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -322,10 +391,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -549,7 +615,7 @@
   <dimension ref="A1:AD1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -571,59 +637,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="11"/>
+      <c r="A1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
     </row>
     <row r="2" spans="1:30" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="16" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="16" t="s">
+      <c r="I2" s="15"/>
+      <c r="J2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="13"/>
+      <c r="K2" s="15"/>
       <c r="L2" s="1" t="s">
         <v>5</v>
       </c>
@@ -657,7 +723,7 @@
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="17"/>
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
@@ -709,42 +775,44 @@
       <c r="AD3" s="3"/>
     </row>
     <row r="4" spans="1:30" ht="187.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19" t="s">
+      <c r="C4" s="20">
+        <v>2</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="11" t="s">
         <v>25</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="11" t="s">
         <v>27</v>
       </c>
       <c r="J4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="11" t="s">
         <v>28</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N4" s="9" t="s">
         <v>29</v>
@@ -766,27 +834,49 @@
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
     </row>
-    <row r="5" spans="1:30" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:30" ht="145.19999999999999" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19" t="s">
-        <v>21</v>
+      <c r="C5" s="20">
+        <v>4</v>
       </c>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
+      <c r="D5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -804,29 +894,49 @@
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
     </row>
-    <row r="6" spans="1:30" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:30" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19" t="s">
-        <v>21</v>
+      <c r="C6" s="20">
+        <v>3</v>
       </c>
-      <c r="M6" s="19" t="s">
-        <v>30</v>
+      <c r="D6" s="9" t="s">
+        <v>45</v>
       </c>
-      <c r="N6" s="19"/>
+      <c r="E6" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
@@ -845,26 +955,48 @@
       <c r="AD6" s="3"/>
     </row>
     <row r="7" spans="1:30" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19" t="s">
-        <v>21</v>
+      <c r="C7" s="20">
+        <v>1</v>
       </c>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
+      <c r="D7" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
@@ -883,26 +1015,22 @@
       <c r="AD7" s="3"/>
     </row>
     <row r="8" spans="1:30" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
@@ -8493,7 +8621,7 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L4:L24" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"in auto/moto,con i mezzi pubblici,a piedi/in bicicletta,soluzione mista: auto/moto + mezzi pubblici,altro da specificare nelle note"</formula1>
     </dataValidation>

</xml_diff>